<commit_message>
Cleared remaining DRC, add JLCPCB part numbers
</commit_message>
<xml_diff>
--- a/kicad/bq25504_Design_Help_V1_2.xlsx
+++ b/kicad/bq25504_Design_Help_V1_2.xlsx
@@ -1328,7 +1328,7 @@
       <xdr:col>2</xdr:col>
       <xdr:colOff>219600</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>15480</xdr:rowOff>
+      <xdr:rowOff>15120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1337,8 +1337,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2644920" y="4143240"/>
-          <a:ext cx="360" cy="298080"/>
+          <a:off x="2143800" y="4143240"/>
+          <a:ext cx="360" cy="297720"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -1390,7 +1390,7 @@
       <xdr:col>8</xdr:col>
       <xdr:colOff>219600</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>53640</xdr:rowOff>
+      <xdr:rowOff>53280</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1399,8 +1399,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7340760" y="4280400"/>
-          <a:ext cx="360" cy="199080"/>
+          <a:off x="5868360" y="4280400"/>
+          <a:ext cx="360" cy="198720"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -1452,7 +1452,7 @@
       <xdr:col>20</xdr:col>
       <xdr:colOff>238320</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>44280</xdr:rowOff>
+      <xdr:rowOff>43920</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1461,8 +1461,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="15683760" y="4480200"/>
-          <a:ext cx="360" cy="180360"/>
+          <a:off x="12489120" y="4480200"/>
+          <a:ext cx="360" cy="180000"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -1512,7 +1512,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>8640</xdr:colOff>
+      <xdr:colOff>8280</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>124200</xdr:rowOff>
     </xdr:to>
@@ -1523,8 +1523,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2435040" y="3191040"/>
-          <a:ext cx="595440" cy="360"/>
+          <a:off x="1933920" y="3191040"/>
+          <a:ext cx="471600" cy="360"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -1573,8 +1573,8 @@
       <xdr:rowOff>114480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>596160</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>123480</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>114840</xdr:rowOff>
     </xdr:to>
@@ -1585,8 +1585,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7121520" y="3181680"/>
-          <a:ext cx="596160" cy="360"/>
+          <a:off x="5649120" y="3181680"/>
+          <a:ext cx="595800" cy="360"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -1636,7 +1636,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>8640</xdr:colOff>
+      <xdr:colOff>8280</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>114840</xdr:rowOff>
     </xdr:to>
@@ -1647,8 +1647,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7130880" y="3400560"/>
-          <a:ext cx="595440" cy="360"/>
+          <a:off x="5658480" y="3400560"/>
+          <a:ext cx="471240" cy="360"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -1698,7 +1698,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>8640</xdr:colOff>
+      <xdr:colOff>8280</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>114840</xdr:rowOff>
     </xdr:to>
@@ -1709,8 +1709,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="15455160" y="3400560"/>
-          <a:ext cx="595440" cy="360"/>
+          <a:off x="12260520" y="3400560"/>
+          <a:ext cx="471240" cy="360"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -1760,9 +1760,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>94680</xdr:colOff>
+      <xdr:colOff>94320</xdr:colOff>
       <xdr:row>65</xdr:row>
-      <xdr:rowOff>82080</xdr:rowOff>
+      <xdr:rowOff>81720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1775,8 +1775,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3815280" y="5690160"/>
-          <a:ext cx="13869360" cy="7076160"/>
+          <a:off x="3030120" y="5690160"/>
+          <a:ext cx="11015640" cy="7075800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1799,7 +1799,7 @@
       <xdr:col>14</xdr:col>
       <xdr:colOff>219600</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>15480</xdr:rowOff>
+      <xdr:rowOff>15120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1808,8 +1808,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11553480" y="4143240"/>
-          <a:ext cx="360" cy="298080"/>
+          <a:off x="9209520" y="4143240"/>
+          <a:ext cx="360" cy="297720"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -1859,7 +1859,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>8640</xdr:colOff>
+      <xdr:colOff>8280</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>124200</xdr:rowOff>
     </xdr:to>
@@ -1870,8 +1870,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11343600" y="3191040"/>
-          <a:ext cx="595440" cy="360"/>
+          <a:off x="8999640" y="3191040"/>
+          <a:ext cx="471240" cy="360"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -1923,7 +1923,7 @@
       <xdr:col>14</xdr:col>
       <xdr:colOff>219600</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>15480</xdr:rowOff>
+      <xdr:rowOff>15120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1932,8 +1932,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11553480" y="4143240"/>
-          <a:ext cx="360" cy="298080"/>
+          <a:off x="9209520" y="4143240"/>
+          <a:ext cx="360" cy="297720"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -1983,7 +1983,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>8640</xdr:colOff>
+      <xdr:colOff>8280</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>124200</xdr:rowOff>
     </xdr:to>
@@ -1994,8 +1994,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11343600" y="3191040"/>
-          <a:ext cx="595440" cy="360"/>
+          <a:off x="8999640" y="3191040"/>
+          <a:ext cx="471240" cy="360"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -2049,29 +2049,29 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="C36" activeCellId="0" sqref="C36"/>
+      <selection pane="topRight" activeCell="AC16" activeCellId="0" sqref="AC16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="6.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="6.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="8.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="6.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="6.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="2.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="19.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="6.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="6.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="0" width="8.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="6.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="6.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="2.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="13.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="6.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="6.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="16" style="0" width="8.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="6.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="6.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="2.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="12.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="6.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="6.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="22" style="0" width="8.7"/>
   </cols>
   <sheetData>
@@ -2860,7 +2860,8 @@
         <v>43</v>
       </c>
       <c r="C20" s="32" t="n">
-        <v>5.23</v>
+        <f aca="false">C19</f>
+        <v>4.99</v>
       </c>
       <c r="D20" s="33" t="s">
         <v>21</v>
@@ -2980,14 +2981,14 @@
       </c>
       <c r="C23" s="57" t="n">
         <f aca="false">$C$1*(1+C20/C19)*3/2</f>
-        <v>3.84018036072144</v>
+        <v>3.75</v>
       </c>
       <c r="D23" s="58" t="s">
         <v>2</v>
       </c>
       <c r="E23" s="59" t="n">
         <f aca="false">(C23-C9)/C23*100</f>
-        <v>-0.54215264187867</v>
+        <v>-2.96000000000001</v>
       </c>
       <c r="F23" s="60" t="s">
         <v>51</v>
@@ -4039,7 +4040,7 @@
       <selection pane="topLeft" activeCell="J32" activeCellId="0" sqref="J32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>